<commit_message>
Agregando nuevas funciones automatizadas
</commit_message>
<xml_diff>
--- a/Data/DataReport.xlsx
+++ b/Data/DataReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BDGSA\Documents\UiPath\DataTableExcelUI\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03DEC29E-BC80-4C68-B792-726B63E3C37C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0A9099-590B-4B02-8E65-F05EBE395CAB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2250" yWindow="480" windowWidth="15375" windowHeight="7875" xr2:uid="{D6C43EA4-6B3E-477B-AEE2-8A3277D45187}"/>
+    <workbookView xWindow="2250" yWindow="480" windowWidth="15375" windowHeight="7875" xr2:uid="{FB841964-9AD3-47BE-879A-A36611A45CB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>YEAR</t>
   </si>
@@ -437,8 +437,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48E12B6C-5EA3-45A0-B5A9-6E461D49896F}">
-  <dimension ref="A1:C15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3653921-853F-4623-AFA9-AE3E25676E8C}">
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -576,39 +576,6 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>1995</v>
-      </c>
-      <c r="B13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>1983</v>
-      </c>
-      <c r="B14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>1980</v>
-      </c>
-      <c r="B15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" t="s">
-        <v>18</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>